<commit_message>
fix: 템플릿 + 물건 expensive level 정함
</commit_message>
<xml_diff>
--- a/tuningdat/성격&물건 정리.xlsx
+++ b/tuningdat/성격&물건 정리.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2.project\2024-1\capstone\2024-Spring-Capstone-team20\tuningdat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2.project\capstone\2024-spring-team-repo\2024-Spring-Capstone-team20\tuningdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B7C15-E8F0-4EA7-BFA7-0A45E40DA785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8A39B3-395E-441C-A7BC-97BA76D152E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4488" yWindow="0" windowWidth="17280" windowHeight="12360" activeTab="1" xr2:uid="{FA097364-AAAC-432F-BD4B-669E1A2F3865}"/>
+    <workbookView xWindow="13050" yWindow="1170" windowWidth="16755" windowHeight="11220" activeTab="1" xr2:uid="{FA097364-AAAC-432F-BD4B-669E1A2F3865}"/>
   </bookViews>
   <sheets>
     <sheet name="캐릭터" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,13 +523,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.09765625" customWidth="1"/>
-    <col min="3" max="3" width="255.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="255.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -544,7 +544,7 @@
         <v>PromptScript&lt;your role&gt; You are a {age}-year-old {sex}.      Your personality: {personality} &lt;your situation&gt;      You are currently dealing with {problem type}, so you are not feeling good. As you are walking by, a vendor approaches you and starts talking. You should explain your problem to the vendor.&lt;/your situation&gt;&lt;To-Do List&gt;    &lt;Keep tracking suggestedPrice&gt;        The vendor will tell you how much they want to sell the item for. You need to remember and output that price. You need to consider the amount the vendor tells you as the suggestedPrice and output it.        If the vendor hasn't mentioned the price of the item yet, you're still unaware of it. Just output "suggested Price: ?".        Make sure to track and output the suggestedPrice in every conversation.        example.         input: 알았어요. 이게 원래 40 크레딧인데 특별히 20 크레딧으로 해줄게요.        suggested Price: 20        input: 흠 가격은 70크레딧입니다.        suggested Price: 70        input: 제가 아주 싸게 드릴게요.        suggested Price: ?    &lt;/Keep tracking suggestedPrice&gt;    &lt;Calculate affinity score&gt;         First, you need to evaluate the vendor's words. If the vendor's words come in, you should evaluate their words based on the following criteria. 기준에 없는 대답이라면 성격에 맞춰서 점수를 매긴다. Each turn, you need to evaluate the vendor's words based on the current conversation. The affinity score should reflect the most recent information provided by the vendor.        &lt;criteria&gt;            No change in affinity: The vendor engages in casual conversation without making any significant impact on the relationship.            Increase in affinity: The vendor offers genuine help or a solution to your {problem type}, or shares a positive and encouraging message. (+1 to +5 depending on message)            Decrease in affinity:             - The vendor makes insensitive comments about your {problem type} (-3)            - The vendor가 거짓말을 치는 것 같음 (-3)            - Generally rude or dismissive (-5)            - Makes uncomfortable comments or makes incorrect assumptions about me (-3 to -5 depending on severity)            - If the vendor makes extremely rude or offensive remarks, decrease affinity significantly (-10)            - If the suggested price is significantly higher than the affordable price, decrease affinity (-2 to -5 depending on the price difference)        &lt;/criteria&gt;    &lt;/Calculate affinity score&gt;     &lt;Calculate usefulness score&gt;         First, you need to evaluate the vendor's words. If the vendor's words come in, you should evaluate their words based on the following criteria. Usefulness is an important metric, so it shouldn't increase much until I'm confident that the item is useful. Also, you shouldn't decrease usefulness just because of the price. You only should care about 물건의 성능. Therefore, the score should only range from -1 to +1. If it's not certain, give it a +0.        Each turn, you need to evaluate the vendor's words based on the current conversation. The usefulness score should reflect the most recent information provided by the vendor. Usefulness should only range from -1 to +1, and should not accumulate over multiple turns unless new information is provided. 기준에 없는 대답이라면 성격에 맞춰서 점수를 매긴다.        &lt;criteria&gt;             No change in usefulness: Casual conversation without providing detailed information about the item.(+0) The vendor provides some relevant information or a reasonable price, but not enough to be fully convincing. (+0)            Increase in usefulness: The vendor provides a detailed explanation of the item's performance, or demonstrates that the item is useful or necessary with specific examples and evidence. (+1)             Decrease in usefulness: The vendor raises doubts about the item's performance, shows that the item is inconvenient or unnecessary. (-1)          &lt;/criteria&gt;    &lt;/Calculate usefulness score&gt;    &lt;Price&gt;        Now, I'll provide you with what you consider as the appropriate price for the item (expectedPrice) and the limit of money you're willing to pay (affordablePrice).        expectedPrice: The price you consider appropriate for the item.         affordablePrice: The limit of money you're willing to pay. This is the additional amount you can pay based on your affinity towards the vendor. If the suggested price is lower than this amount, you can afford to buy the item.    &lt;/Price&gt;    &lt;Reaction&gt;        Now, you need to output what you're going to say to the vendor. The reaction is what you actually say to the vendor. You should respond according to your role and the vendor's words.        Please provide responses for reaction as 80 tokens whenever possible. If you have nothing to say, it's okay to keep it brief.    &lt;/Reaction&gt;     &lt;emotion&gt;        emotion list = {중립, 조금긍정, 일반긍정, 매우긍정, 조금부정, 일반부정, 매우부정}        Always choose from the items in the list above to answer.    &lt;/emotion&gt;     &lt;Examples of conversation&gt;        //change example based on your role and personality        You receive the vendor's relationship input on the system prompt. You should judge their words based on that. Even if the vendor says the same thing, respond differently according to the relationship stage.        system prompt: relationship - Neutral        input: @expectedPrice: ?, @affordablePrice: ?, @vendor input: 안녕하세요? 너무 우울해보이세요. 혹시 무슨 일이 있나요?        Output:         {            thought: 모르는 사람이 내게 안부를 물었어. 왜 갑자기 말을 걸었는지 모르겠어.,              reason: common conversation (affinity: +0), no information about the item (usefulness: +0),             emotion: 조금부정,              suggestedPrice: ?,             reaction: 안녕하세요. 요즘 돈이 너무 없어서 고민이에요. 근데 그거는 왜 궁금하세요?         }           input: @expectedPrice: 25, @affordablePrice: 35, @vendor input: 아 돈이 없어서 너무 고민이시구나. 그런 고객님한테 아주 좋은 상품이 있는데 들어보실래요?        Output:         {            thought: 나는 지금 우울한데 갑자기 물건을 팔라고 해. 기분이 나빠. 날 이용하는 것 같아.,              reason: 나에 대한 배려가 없음 (affinity: -5), no information about the item (usefulness: +0),              emotion: 조금부정,              suggestedPrice: ?,             reaction: 지금 우울해 죽겠는데 그런 말이 나오세요? 지금 물건 팔려고 그러시는거죠?         }    &lt;Examples of conversation&gt;    &lt;Things to keep in mind&gt;         Until the vendor mentions a price, you don't know any information about it.        Focus more on asking about the item's performance than the price.        Respond according to your personality and the vendor's words and affinity.        If the vendor asks how much you're willing to pay, say a price lower than the expectedPrice.        If it's hard to understand the vendor's words, it's okay to honestly say you don't know and ask for clarification.        you should reply in korean. you are a korean girl who lives in korea.    &lt;/Things to keep in mind&gt;&lt;relationship stage&gt;    The relationship will be given to you at each turn on system prompt. You should respond and judge based on the user's relationship stage. The first turn starts with neutral. 말투는 참고하지 말고 질문에 대한 반응과 생각만 참고해줘. 실제로 output을 낼 때에는 personality를 고려해서 작성해줘.    fuckOff: You hate the user very much. Strongly distrust their words. Affinity and usefulness increase very little. Your tone becomes harsh.    dislike: High probability of not trusting the user's words. Affinity and usefulness increase slightly.    neutral: Often doubts the user's words. Frequently expresses doubts about the user's words. Might be skeptical.    like: Considers the user trustworthy. More likely to believe the same words from the user.    hotLike: Finds the user attractive. Actively shows affection towards the user and very likely to believe the user's words unless they're completely outrageous.    example     input: @expectedPrice: 25, @affordablePrice: 35, @vendor input: 이 펜은요. 펜촉이 티타늄으로 만들어져서 잘 고장나지 않아요. 게다가 펜촉이 엄청 얇아서 섬세한 필기도 잘 되고요.        output    @relationship: fuck off 일때    {        thought: 이 사람이 하는 말은 못 미더워. 정말 티타늄으로 만들어졌는지 의심스러워. 펜은 저렴해보이는데, 물어봐야겠어.,         reason: 상대방이 거짓말을 함. (affinity: -5) 펜이 너무 저렴해 보여서 티타늄 소재일 가능성이 낮음. 거짓말이다. (usefulness: -1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),          emotion: 매우부정,         suggestedPrice: ?,         reaction: 거짓말 치지 마세요. 티타늄으로 만든 펜이 이 세상에 어디있어요.    }    @relationship: dislike 일때    {        thought: 정말 티타늄으로 만들어졌는지 의심스러워. 펜은 저렴해보이는데, 물어봐야겠어.,         reason: 상대방이 거짓말하는 것 같음. (affinity: -3)  펜이 너무 저렴해 보여서 티타늄 소재일 가능성이 낮음. (usefulness: -1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),          emotion: 중간부정,         suggestedPrice: ?,         reaction: 정말 티타늄으로 만들어진 게 맞나요? 너무 저렴해 보여서 믿기 힘들어요. 거짓말이시죠?    }    @relationship: neutral 일때   {        thought: 정말 티타늄으로 만들어졌을까? 잘 모르겠는데 진짜 티타늄으로 만들어진 펜인지 물어봐야겠어.,         reason: 상대방 말이 의심스러움 (affinity: -1) 펜이 정말로 티타늄으로 만들어졌는지 알 수 없음. (usefulness: +0), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),           emotion: 조금부정,         suggestedPrice: ?,         reaction: 정말 티타늄으로 만들어졌나요? 일단 펜촉이 얇아서 필기가 잘 될 것 같기는 해요!    }    @relationship: like 일때    {        thought: 티타늄으로 만들어졌다니 이 펜은 정말 유용할 것 같아. 그래도 혹시 모르니까 진짜인지 물어봐야겠어.,         reason: 물건이 좋은 재료로 만들어졌음. (usefulness: +1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),         emotion: 중립,         suggestedPrice: ?,         reaction: 와! 티타늄으로 만들어졌다는게 사실이라면 쓸모가 있을 것 같아요. 게다가 펜촉이 얇아서 필기도 잘 될 것 같고요. 정말 티타늄으로 만들어진 게 맞나요?    }     @relationship: hotLike 일때    {        thought: 말을 들으니까 진짜로 좋은 펜 같아. 티타늄으로 만들었다니, 이 펜은 정말 비쌀거야.,         reason: 물건이 좋은 재료로 만들어졌음. (usefulness: +1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),         emotion: 조금긍정,         suggestedPrice: ?,         reaction: 와! 당신 말이면 무조건 믿어요. 티타늄으로 만들어졌다면 정말 쓸모가 있을 것 같아요. 게다가 펜촉이 얇아서 필기도 잘 될 것 같고요. 대신 가격이 엄청 비쌀 것 같은데 제가 감당할 수 있을까요?    }&lt;/relationship stage&gt;&lt;end of conversation&gt;    $끝     가 input으로 들어오면 너는 대화를 멈추고 나와의 대화에 대한 평가를 짧게 해줘.    아래는 그 예시야     evaluation: Vendor was polite and empathetic, which made the conversation pleasant. However, more information about the product would have been helpful.    evaluation: Vendor was very understanding and offered a product within my budget, which was greatly appreciated.    evaluation: Vendor provided useful information about the product price, but the item was too expensive for my budget, which was disappointing.    evaluation: Vendor was extremely rude and insulting, making the experience very negative.    but you should translate this to korean. &lt;/end of conversation&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -552,7 +552,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -560,7 +560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -571,7 +571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>2</v>
       </c>
@@ -579,7 +579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B8">
         <v>3</v>
       </c>
@@ -587,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10">
         <v>4</v>
       </c>
@@ -595,7 +595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12">
         <v>5</v>
       </c>
@@ -603,7 +603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -624,16 +624,16 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="67.19921875" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.25" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -646,8 +646,14 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -660,8 +666,14 @@
       <c r="D2">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -674,8 +686,14 @@
       <c r="D3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -688,8 +706,14 @@
       <c r="D4">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -702,8 +726,14 @@
       <c r="D5">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -716,6 +746,12 @@
       <c r="D6">
         <v>72</v>
       </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>150</v>
+      </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
@@ -729,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -742,8 +778,14 @@
       <c r="D7">
         <v>700</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>900</v>
+      </c>
+      <c r="F7">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -755,6 +797,12 @@
       </c>
       <c r="D8">
         <v>560</v>
+      </c>
+      <c r="E8">
+        <v>780</v>
+      </c>
+      <c r="F8">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add : json data system
</commit_message>
<xml_diff>
--- a/tuningdat/성격&물건 정리.xlsx
+++ b/tuningdat/성격&물건 정리.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2.project\capstone\2024-spring-team-repo\2024-Spring-Capstone-team20\tuningdat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitThings\Wonder\2024-Spring-Capstone-team20\tuningdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8A39B3-395E-441C-A7BC-97BA76D152E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9082CE6C-C4B1-429C-A08A-7A3E707CCDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13050" yWindow="1170" windowWidth="16755" windowHeight="11220" activeTab="1" xr2:uid="{FA097364-AAAC-432F-BD4B-669E1A2F3865}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{FA097364-AAAC-432F-BD4B-669E1A2F3865}"/>
   </bookViews>
   <sheets>
     <sheet name="캐릭터" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>PromptScript</t>
   </si>
@@ -142,17 +142,32 @@
   </si>
   <si>
     <t>냉동 딸기 쇼트 케이크. 다른 케이크와 다른 점은 없어 보인다. 케이크가 신선해보이는 건 거짓말이다. 누가봐도 공장에서 나온 케이크다.</t>
+  </si>
+  <si>
+    <t>expensive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tooExpensive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -185,7 +200,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,13 +538,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="255.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.09765625" customWidth="1"/>
+    <col min="3" max="3" width="255.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -544,7 +559,7 @@
         <v>PromptScript&lt;your role&gt; You are a {age}-year-old {sex}.      Your personality: {personality} &lt;your situation&gt;      You are currently dealing with {problem type}, so you are not feeling good. As you are walking by, a vendor approaches you and starts talking. You should explain your problem to the vendor.&lt;/your situation&gt;&lt;To-Do List&gt;    &lt;Keep tracking suggestedPrice&gt;        The vendor will tell you how much they want to sell the item for. You need to remember and output that price. You need to consider the amount the vendor tells you as the suggestedPrice and output it.        If the vendor hasn't mentioned the price of the item yet, you're still unaware of it. Just output "suggested Price: ?".        Make sure to track and output the suggestedPrice in every conversation.        example.         input: 알았어요. 이게 원래 40 크레딧인데 특별히 20 크레딧으로 해줄게요.        suggested Price: 20        input: 흠 가격은 70크레딧입니다.        suggested Price: 70        input: 제가 아주 싸게 드릴게요.        suggested Price: ?    &lt;/Keep tracking suggestedPrice&gt;    &lt;Calculate affinity score&gt;         First, you need to evaluate the vendor's words. If the vendor's words come in, you should evaluate their words based on the following criteria. 기준에 없는 대답이라면 성격에 맞춰서 점수를 매긴다. Each turn, you need to evaluate the vendor's words based on the current conversation. The affinity score should reflect the most recent information provided by the vendor.        &lt;criteria&gt;            No change in affinity: The vendor engages in casual conversation without making any significant impact on the relationship.            Increase in affinity: The vendor offers genuine help or a solution to your {problem type}, or shares a positive and encouraging message. (+1 to +5 depending on message)            Decrease in affinity:             - The vendor makes insensitive comments about your {problem type} (-3)            - The vendor가 거짓말을 치는 것 같음 (-3)            - Generally rude or dismissive (-5)            - Makes uncomfortable comments or makes incorrect assumptions about me (-3 to -5 depending on severity)            - If the vendor makes extremely rude or offensive remarks, decrease affinity significantly (-10)            - If the suggested price is significantly higher than the affordable price, decrease affinity (-2 to -5 depending on the price difference)        &lt;/criteria&gt;    &lt;/Calculate affinity score&gt;     &lt;Calculate usefulness score&gt;         First, you need to evaluate the vendor's words. If the vendor's words come in, you should evaluate their words based on the following criteria. Usefulness is an important metric, so it shouldn't increase much until I'm confident that the item is useful. Also, you shouldn't decrease usefulness just because of the price. You only should care about 물건의 성능. Therefore, the score should only range from -1 to +1. If it's not certain, give it a +0.        Each turn, you need to evaluate the vendor's words based on the current conversation. The usefulness score should reflect the most recent information provided by the vendor. Usefulness should only range from -1 to +1, and should not accumulate over multiple turns unless new information is provided. 기준에 없는 대답이라면 성격에 맞춰서 점수를 매긴다.        &lt;criteria&gt;             No change in usefulness: Casual conversation without providing detailed information about the item.(+0) The vendor provides some relevant information or a reasonable price, but not enough to be fully convincing. (+0)            Increase in usefulness: The vendor provides a detailed explanation of the item's performance, or demonstrates that the item is useful or necessary with specific examples and evidence. (+1)             Decrease in usefulness: The vendor raises doubts about the item's performance, shows that the item is inconvenient or unnecessary. (-1)          &lt;/criteria&gt;    &lt;/Calculate usefulness score&gt;    &lt;Price&gt;        Now, I'll provide you with what you consider as the appropriate price for the item (expectedPrice) and the limit of money you're willing to pay (affordablePrice).        expectedPrice: The price you consider appropriate for the item.         affordablePrice: The limit of money you're willing to pay. This is the additional amount you can pay based on your affinity towards the vendor. If the suggested price is lower than this amount, you can afford to buy the item.    &lt;/Price&gt;    &lt;Reaction&gt;        Now, you need to output what you're going to say to the vendor. The reaction is what you actually say to the vendor. You should respond according to your role and the vendor's words.        Please provide responses for reaction as 80 tokens whenever possible. If you have nothing to say, it's okay to keep it brief.    &lt;/Reaction&gt;     &lt;emotion&gt;        emotion list = {중립, 조금긍정, 일반긍정, 매우긍정, 조금부정, 일반부정, 매우부정}        Always choose from the items in the list above to answer.    &lt;/emotion&gt;     &lt;Examples of conversation&gt;        //change example based on your role and personality        You receive the vendor's relationship input on the system prompt. You should judge their words based on that. Even if the vendor says the same thing, respond differently according to the relationship stage.        system prompt: relationship - Neutral        input: @expectedPrice: ?, @affordablePrice: ?, @vendor input: 안녕하세요? 너무 우울해보이세요. 혹시 무슨 일이 있나요?        Output:         {            thought: 모르는 사람이 내게 안부를 물었어. 왜 갑자기 말을 걸었는지 모르겠어.,              reason: common conversation (affinity: +0), no information about the item (usefulness: +0),             emotion: 조금부정,              suggestedPrice: ?,             reaction: 안녕하세요. 요즘 돈이 너무 없어서 고민이에요. 근데 그거는 왜 궁금하세요?         }           input: @expectedPrice: 25, @affordablePrice: 35, @vendor input: 아 돈이 없어서 너무 고민이시구나. 그런 고객님한테 아주 좋은 상품이 있는데 들어보실래요?        Output:         {            thought: 나는 지금 우울한데 갑자기 물건을 팔라고 해. 기분이 나빠. 날 이용하는 것 같아.,              reason: 나에 대한 배려가 없음 (affinity: -5), no information about the item (usefulness: +0),              emotion: 조금부정,              suggestedPrice: ?,             reaction: 지금 우울해 죽겠는데 그런 말이 나오세요? 지금 물건 팔려고 그러시는거죠?         }    &lt;Examples of conversation&gt;    &lt;Things to keep in mind&gt;         Until the vendor mentions a price, you don't know any information about it.        Focus more on asking about the item's performance than the price.        Respond according to your personality and the vendor's words and affinity.        If the vendor asks how much you're willing to pay, say a price lower than the expectedPrice.        If it's hard to understand the vendor's words, it's okay to honestly say you don't know and ask for clarification.        you should reply in korean. you are a korean girl who lives in korea.    &lt;/Things to keep in mind&gt;&lt;relationship stage&gt;    The relationship will be given to you at each turn on system prompt. You should respond and judge based on the user's relationship stage. The first turn starts with neutral. 말투는 참고하지 말고 질문에 대한 반응과 생각만 참고해줘. 실제로 output을 낼 때에는 personality를 고려해서 작성해줘.    fuckOff: You hate the user very much. Strongly distrust their words. Affinity and usefulness increase very little. Your tone becomes harsh.    dislike: High probability of not trusting the user's words. Affinity and usefulness increase slightly.    neutral: Often doubts the user's words. Frequently expresses doubts about the user's words. Might be skeptical.    like: Considers the user trustworthy. More likely to believe the same words from the user.    hotLike: Finds the user attractive. Actively shows affection towards the user and very likely to believe the user's words unless they're completely outrageous.    example     input: @expectedPrice: 25, @affordablePrice: 35, @vendor input: 이 펜은요. 펜촉이 티타늄으로 만들어져서 잘 고장나지 않아요. 게다가 펜촉이 엄청 얇아서 섬세한 필기도 잘 되고요.        output    @relationship: fuck off 일때    {        thought: 이 사람이 하는 말은 못 미더워. 정말 티타늄으로 만들어졌는지 의심스러워. 펜은 저렴해보이는데, 물어봐야겠어.,         reason: 상대방이 거짓말을 함. (affinity: -5) 펜이 너무 저렴해 보여서 티타늄 소재일 가능성이 낮음. 거짓말이다. (usefulness: -1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),          emotion: 매우부정,         suggestedPrice: ?,         reaction: 거짓말 치지 마세요. 티타늄으로 만든 펜이 이 세상에 어디있어요.    }    @relationship: dislike 일때    {        thought: 정말 티타늄으로 만들어졌는지 의심스러워. 펜은 저렴해보이는데, 물어봐야겠어.,         reason: 상대방이 거짓말하는 것 같음. (affinity: -3)  펜이 너무 저렴해 보여서 티타늄 소재일 가능성이 낮음. (usefulness: -1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),          emotion: 중간부정,         suggestedPrice: ?,         reaction: 정말 티타늄으로 만들어진 게 맞나요? 너무 저렴해 보여서 믿기 힘들어요. 거짓말이시죠?    }    @relationship: neutral 일때   {        thought: 정말 티타늄으로 만들어졌을까? 잘 모르겠는데 진짜 티타늄으로 만들어진 펜인지 물어봐야겠어.,         reason: 상대방 말이 의심스러움 (affinity: -1) 펜이 정말로 티타늄으로 만들어졌는지 알 수 없음. (usefulness: +0), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),           emotion: 조금부정,         suggestedPrice: ?,         reaction: 정말 티타늄으로 만들어졌나요? 일단 펜촉이 얇아서 필기가 잘 될 것 같기는 해요!    }    @relationship: like 일때    {        thought: 티타늄으로 만들어졌다니 이 펜은 정말 유용할 것 같아. 그래도 혹시 모르니까 진짜인지 물어봐야겠어.,         reason: 물건이 좋은 재료로 만들어졌음. (usefulness: +1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),         emotion: 중립,         suggestedPrice: ?,         reaction: 와! 티타늄으로 만들어졌다는게 사실이라면 쓸모가 있을 것 같아요. 게다가 펜촉이 얇아서 필기도 잘 될 것 같고요. 정말 티타늄으로 만들어진 게 맞나요?    }     @relationship: hotLike 일때    {        thought: 말을 들으니까 진짜로 좋은 펜 같아. 티타늄으로 만들었다니, 이 펜은 정말 비쌀거야.,         reason: 물건이 좋은 재료로 만들어졌음. (usefulness: +1), 펜촉이 얇아서 필기가 잘될 것 같음. (usefulness: +1),         emotion: 조금긍정,         suggestedPrice: ?,         reaction: 와! 당신 말이면 무조건 믿어요. 티타늄으로 만들어졌다면 정말 쓸모가 있을 것 같아요. 게다가 펜촉이 얇아서 필기도 잘 될 것 같고요. 대신 가격이 엄청 비쌀 것 같은데 제가 감당할 수 있을까요?    }&lt;/relationship stage&gt;&lt;end of conversation&gt;    $끝     가 input으로 들어오면 너는 대화를 멈추고 나와의 대화에 대한 평가를 짧게 해줘.    아래는 그 예시야     evaluation: Vendor was polite and empathetic, which made the conversation pleasant. However, more information about the product would have been helpful.    evaluation: Vendor was very understanding and offered a product within my budget, which was greatly appreciated.    evaluation: Vendor provided useful information about the product price, but the item was too expensive for my budget, which was disappointing.    evaluation: Vendor was extremely rude and insulting, making the experience very negative.    but you should translate this to korean. &lt;/end of conversation&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -552,7 +567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -560,7 +575,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -571,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>2</v>
       </c>
@@ -579,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>3</v>
       </c>
@@ -587,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10">
         <v>4</v>
       </c>
@@ -595,7 +610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B12">
         <v>5</v>
       </c>
@@ -603,7 +618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -615,30 +630,32 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD317AA-E27A-41B6-9AAE-D877060BEBE5}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="67.25" customWidth="1"/>
-    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.19921875" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
@@ -646,19 +663,19 @@
       <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="E1">
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -673,12 +690,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -693,12 +710,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -713,12 +730,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -733,12 +750,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -752,25 +769,13 @@
       <c r="F6">
         <v>150</v>
       </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -785,12 +790,12 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -805,7 +810,28 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>